<commit_message>
Change dataset estimados legisladores municipales
</commit_message>
<xml_diff>
--- a/output/total_legisladores_municipales.xlsx
+++ b/output/total_legisladores_municipales.xlsx
@@ -636,7 +636,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>17929</v>
+        <v>18020</v>
       </c>
       <c r="C2" s="2">
         <v>12</v>
@@ -647,7 +647,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>37866</v>
+        <v>38136</v>
       </c>
       <c r="C3" s="2">
         <v>14</v>
@@ -658,7 +658,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>54056</v>
+        <v>55101</v>
       </c>
       <c r="C4" s="2">
         <v>16</v>
@@ -669,7 +669,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="2">
-        <v>24013</v>
+        <v>24223</v>
       </c>
       <c r="C5" s="2">
         <v>14</v>
@@ -680,7 +680,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2">
-        <v>24528</v>
+        <v>24637</v>
       </c>
       <c r="C6" s="2">
         <v>14</v>
@@ -691,7 +691,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="2">
-        <v>25360</v>
+        <v>25596</v>
       </c>
       <c r="C7" s="2">
         <v>14</v>
@@ -702,7 +702,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="2">
-        <v>86287</v>
+        <v>87754</v>
       </c>
       <c r="C8" s="2">
         <v>16</v>
@@ -713,7 +713,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="2">
-        <v>15774</v>
+        <v>15843</v>
       </c>
       <c r="C9" s="2">
         <v>12</v>
@@ -724,7 +724,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2">
-        <v>22590</v>
+        <v>22657</v>
       </c>
       <c r="C10" s="2">
         <v>14</v>
@@ -735,7 +735,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="2">
-        <v>28717</v>
+        <v>28983</v>
       </c>
       <c r="C11" s="2">
         <v>14</v>
@@ -746,7 +746,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="2">
-        <v>179387</v>
+        <v>185187</v>
       </c>
       <c r="C12" s="2">
         <v>16</v>
@@ -757,7 +757,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="2">
-        <v>46790</v>
+        <v>47158</v>
       </c>
       <c r="C13" s="2">
         <v>16</v>
@@ -768,7 +768,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="2">
-        <v>125961</v>
+        <v>127244</v>
       </c>
       <c r="C14" s="2">
         <v>16</v>
@@ -779,7 +779,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="2">
-        <v>32541</v>
+        <v>32827</v>
       </c>
       <c r="C15" s="2">
         <v>14</v>
@@ -790,7 +790,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="2">
-        <v>42034</v>
+        <v>42337</v>
       </c>
       <c r="C16" s="2">
         <v>16</v>
@@ -801,7 +801,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="2">
-        <v>153371</v>
+        <v>154815</v>
       </c>
       <c r="C17" s="2">
         <v>16</v>
@@ -812,7 +812,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="2">
-        <v>23025</v>
+        <v>23155</v>
       </c>
       <c r="C18" s="2">
         <v>14</v>
@@ -823,7 +823,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="2">
-        <v>41481</v>
+        <v>41652</v>
       </c>
       <c r="C19" s="2">
         <v>16</v>
@@ -834,7 +834,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="2">
-        <v>11181</v>
+        <v>11307</v>
       </c>
       <c r="C20" s="2">
         <v>12</v>
@@ -845,7 +845,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="2">
-        <v>16872</v>
+        <v>16984</v>
       </c>
       <c r="C21" s="2">
         <v>12</v>
@@ -856,7 +856,7 @@
         <v>23</v>
       </c>
       <c r="B22" s="2">
-        <v>39700</v>
+        <v>39970</v>
       </c>
       <c r="C22" s="2">
         <v>14</v>
@@ -867,7 +867,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="2">
-        <v>34435</v>
+        <v>34668</v>
       </c>
       <c r="C23" s="2">
         <v>14</v>
@@ -878,7 +878,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="2">
-        <v>18806</v>
+        <v>18883</v>
       </c>
       <c r="C24" s="2">
         <v>12</v>
@@ -889,7 +889,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="2">
-        <v>34257</v>
+        <v>34571</v>
       </c>
       <c r="C25" s="2">
         <v>14</v>
@@ -900,7 +900,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="2">
-        <v>1182</v>
+        <v>1792</v>
       </c>
       <c r="C26" s="2">
         <v>5</v>
@@ -911,7 +911,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="2">
-        <v>35717</v>
+        <v>35879</v>
       </c>
       <c r="C27" s="2">
         <v>14</v>
@@ -922,7 +922,7 @@
         <v>29</v>
       </c>
       <c r="B28" s="2">
-        <v>31852</v>
+        <v>32124</v>
       </c>
       <c r="C28" s="2">
         <v>14</v>
@@ -933,7 +933,7 @@
         <v>30</v>
       </c>
       <c r="B29" s="2">
-        <v>11614</v>
+        <v>11692</v>
       </c>
       <c r="C29" s="2">
         <v>12</v>
@@ -944,7 +944,7 @@
         <v>31</v>
       </c>
       <c r="B30" s="2">
-        <v>13527</v>
+        <v>13787</v>
       </c>
       <c r="C30" s="2">
         <v>12</v>
@@ -955,7 +955,7 @@
         <v>32</v>
       </c>
       <c r="B31" s="2">
-        <v>33948</v>
+        <v>36614</v>
       </c>
       <c r="C31" s="2">
         <v>14</v>
@@ -966,7 +966,7 @@
         <v>33</v>
       </c>
       <c r="B32" s="2">
-        <v>17590</v>
+        <v>17784</v>
       </c>
       <c r="C32" s="2">
         <v>12</v>
@@ -977,7 +977,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="2">
-        <v>89178</v>
+        <v>89780</v>
       </c>
       <c r="C33" s="2">
         <v>16</v>
@@ -988,7 +988,7 @@
         <v>35</v>
       </c>
       <c r="B34" s="2">
-        <v>40331</v>
+        <v>40622</v>
       </c>
       <c r="C34" s="2">
         <v>16</v>
@@ -999,7 +999,7 @@
         <v>36</v>
       </c>
       <c r="B35" s="2">
-        <v>38219</v>
+        <v>38486</v>
       </c>
       <c r="C35" s="2">
         <v>14</v>
@@ -1010,7 +1010,7 @@
         <v>37</v>
       </c>
       <c r="B36" s="2">
-        <v>15477</v>
+        <v>15654</v>
       </c>
       <c r="C36" s="2">
         <v>12</v>
@@ -1021,7 +1021,7 @@
         <v>38</v>
       </c>
       <c r="B37" s="2">
-        <v>50410</v>
+        <v>50896</v>
       </c>
       <c r="C37" s="2">
         <v>16</v>
@@ -1032,7 +1032,7 @@
         <v>39</v>
       </c>
       <c r="B38" s="2">
-        <v>42415</v>
+        <v>42943</v>
       </c>
       <c r="C38" s="2">
         <v>16</v>
@@ -1043,7 +1043,7 @@
         <v>40</v>
       </c>
       <c r="B39" s="2">
-        <v>14691</v>
+        <v>14779</v>
       </c>
       <c r="C39" s="2">
         <v>12</v>
@@ -1054,7 +1054,7 @@
         <v>41</v>
       </c>
       <c r="B40" s="2">
-        <v>45939</v>
+        <v>46538</v>
       </c>
       <c r="C40" s="2">
         <v>16</v>
@@ -1065,7 +1065,7 @@
         <v>42</v>
       </c>
       <c r="B41" s="2">
-        <v>36868</v>
+        <v>37012</v>
       </c>
       <c r="C41" s="2">
         <v>14</v>
@@ -1076,7 +1076,7 @@
         <v>43</v>
       </c>
       <c r="B42" s="2">
-        <v>23152</v>
+        <v>23334</v>
       </c>
       <c r="C42" s="2">
         <v>14</v>
@@ -1087,7 +1087,7 @@
         <v>44</v>
       </c>
       <c r="B43" s="2">
-        <v>27679</v>
+        <v>28105</v>
       </c>
       <c r="C43" s="2">
         <v>14</v>
@@ -1098,7 +1098,7 @@
         <v>45</v>
       </c>
       <c r="B44" s="2">
-        <v>8752</v>
+        <v>8874</v>
       </c>
       <c r="C44" s="2">
         <v>12</v>
@@ -1109,7 +1109,7 @@
         <v>46</v>
       </c>
       <c r="B45" s="2">
-        <v>35044</v>
+        <v>35180</v>
       </c>
       <c r="C45" s="2">
         <v>14</v>
@@ -1120,7 +1120,7 @@
         <v>47</v>
       </c>
       <c r="B46" s="2">
-        <v>23537</v>
+        <v>23693</v>
       </c>
       <c r="C46" s="2">
         <v>14</v>
@@ -1131,7 +1131,7 @@
         <v>48</v>
       </c>
       <c r="B47" s="2">
-        <v>17681</v>
+        <v>17781</v>
       </c>
       <c r="C47" s="2">
         <v>12</v>
@@ -1142,7 +1142,7 @@
         <v>49</v>
       </c>
       <c r="B48" s="2">
-        <v>39078</v>
+        <v>39492</v>
       </c>
       <c r="C48" s="2">
         <v>14</v>
@@ -1153,7 +1153,7 @@
         <v>50</v>
       </c>
       <c r="B49" s="2">
-        <v>5354</v>
+        <v>4755</v>
       </c>
       <c r="C49" s="2">
         <v>12</v>
@@ -1164,7 +1164,7 @@
         <v>51</v>
       </c>
       <c r="B50" s="2">
-        <v>10556</v>
+        <v>10589</v>
       </c>
       <c r="C50" s="2">
         <v>12</v>
@@ -1175,7 +1175,7 @@
         <v>52</v>
       </c>
       <c r="B51" s="2">
-        <v>71671</v>
+        <v>73077</v>
       </c>
       <c r="C51" s="2">
         <v>16</v>
@@ -1186,7 +1186,7 @@
         <v>53</v>
       </c>
       <c r="B52" s="2">
-        <v>37179</v>
+        <v>37460</v>
       </c>
       <c r="C52" s="2">
         <v>14</v>
@@ -1197,7 +1197,7 @@
         <v>54</v>
       </c>
       <c r="B53" s="2">
-        <v>28603</v>
+        <v>28727</v>
       </c>
       <c r="C53" s="2">
         <v>14</v>
@@ -1208,7 +1208,7 @@
         <v>55</v>
       </c>
       <c r="B54" s="2">
-        <v>23267</v>
+        <v>23386</v>
       </c>
       <c r="C54" s="2">
         <v>14</v>
@@ -1219,7 +1219,7 @@
         <v>56</v>
       </c>
       <c r="B55" s="2">
-        <v>29085</v>
+        <v>29241</v>
       </c>
       <c r="C55" s="2">
         <v>14</v>
@@ -1230,7 +1230,7 @@
         <v>57</v>
       </c>
       <c r="B56" s="2">
-        <v>21240</v>
+        <v>21434</v>
       </c>
       <c r="C56" s="2">
         <v>14</v>
@@ -1241,7 +1241,7 @@
         <v>58</v>
       </c>
       <c r="B57" s="2">
-        <v>15913</v>
+        <v>15985</v>
       </c>
       <c r="C57" s="2">
         <v>12</v>
@@ -1252,7 +1252,7 @@
         <v>59</v>
       </c>
       <c r="B58" s="2">
-        <v>20273</v>
+        <v>20399</v>
       </c>
       <c r="C58" s="2">
         <v>14</v>
@@ -1263,7 +1263,7 @@
         <v>60</v>
       </c>
       <c r="B59" s="2">
-        <v>133340</v>
+        <v>137491</v>
       </c>
       <c r="C59" s="2">
         <v>16</v>
@@ -1274,7 +1274,7 @@
         <v>61</v>
       </c>
       <c r="B60" s="2">
-        <v>23483</v>
+        <v>23638</v>
       </c>
       <c r="C60" s="2">
         <v>14</v>
@@ -1285,7 +1285,7 @@
         <v>62</v>
       </c>
       <c r="B61" s="2">
-        <v>15123</v>
+        <v>15187</v>
       </c>
       <c r="C61" s="2">
         <v>12</v>
@@ -1296,7 +1296,7 @@
         <v>63</v>
       </c>
       <c r="B62" s="2">
-        <v>46323</v>
+        <v>47060</v>
       </c>
       <c r="C62" s="2">
         <v>16</v>
@@ -1307,7 +1307,7 @@
         <v>64</v>
       </c>
       <c r="B63" s="2">
-        <v>22497</v>
+        <v>22729</v>
       </c>
       <c r="C63" s="2">
         <v>14</v>
@@ -1318,7 +1318,7 @@
         <v>65</v>
       </c>
       <c r="B64" s="2">
-        <v>25549</v>
+        <v>25789</v>
       </c>
       <c r="C64" s="2">
         <v>14</v>
@@ -1329,7 +1329,7 @@
         <v>66</v>
       </c>
       <c r="B65" s="2">
-        <v>31269</v>
+        <v>31879</v>
       </c>
       <c r="C65" s="2">
         <v>14</v>
@@ -1340,7 +1340,7 @@
         <v>67</v>
       </c>
       <c r="B66" s="2">
-        <v>335621</v>
+        <v>342259</v>
       </c>
       <c r="C66" s="2">
         <v>17</v>
@@ -1351,7 +1351,7 @@
         <v>68</v>
       </c>
       <c r="B67" s="2">
-        <v>37469</v>
+        <v>37693</v>
       </c>
       <c r="C67" s="2">
         <v>14</v>
@@ -1362,7 +1362,7 @@
         <v>69</v>
       </c>
       <c r="B68" s="2">
-        <v>38993</v>
+        <v>39345</v>
       </c>
       <c r="C68" s="2">
         <v>14</v>
@@ -1373,7 +1373,7 @@
         <v>70</v>
       </c>
       <c r="B69" s="2">
-        <v>20196</v>
+        <v>20281</v>
       </c>
       <c r="C69" s="2">
         <v>14</v>
@@ -1384,7 +1384,7 @@
         <v>71</v>
       </c>
       <c r="B70" s="2">
-        <v>66493</v>
+        <v>66852</v>
       </c>
       <c r="C70" s="2">
         <v>16</v>
@@ -1395,7 +1395,7 @@
         <v>72</v>
       </c>
       <c r="B71" s="2">
-        <v>74410</v>
+        <v>75293</v>
       </c>
       <c r="C71" s="2">
         <v>16</v>
@@ -1406,7 +1406,7 @@
         <v>73</v>
       </c>
       <c r="B72" s="2">
-        <v>67158</v>
+        <v>67740</v>
       </c>
       <c r="C72" s="2">
         <v>16</v>
@@ -1417,7 +1417,7 @@
         <v>74</v>
       </c>
       <c r="B73" s="2">
-        <v>28034</v>
+        <v>28287</v>
       </c>
       <c r="C73" s="2">
         <v>14</v>
@@ -1428,7 +1428,7 @@
         <v>75</v>
       </c>
       <c r="B74" s="2">
-        <v>34960</v>
+        <v>35395</v>
       </c>
       <c r="C74" s="2">
         <v>14</v>
@@ -1439,7 +1439,7 @@
         <v>76</v>
       </c>
       <c r="B75" s="2">
-        <v>53847</v>
+        <v>54414</v>
       </c>
       <c r="C75" s="2">
         <v>16</v>
@@ -1450,7 +1450,7 @@
         <v>77</v>
       </c>
       <c r="B76" s="2">
-        <v>8199</v>
+        <v>8249</v>
       </c>
       <c r="C76" s="2">
         <v>12</v>
@@ -1461,7 +1461,7 @@
         <v>78</v>
       </c>
       <c r="B77" s="2">
-        <v>21858</v>
+        <v>22093</v>
       </c>
       <c r="C77" s="2">
         <v>14</v>
@@ -1472,7 +1472,7 @@
         <v>79</v>
       </c>
       <c r="B78" s="2">
-        <v>30293</v>
+        <v>30426</v>
       </c>
       <c r="C78" s="2">
         <v>14</v>
@@ -1483,7 +1483,7 @@
         <v>80</v>
       </c>
       <c r="B79" s="2">
-        <v>33818</v>
+        <v>34172</v>
       </c>
       <c r="C79" s="2">
         <v>14</v>

</xml_diff>